<commit_message>
thêm cột học kì cho file import, làm chức năg export. chưa format đc, hiện h đang ormat date nên nó bị lỗi. format qua general thì ok, chưa làm chức năng chọn học kì khi import, sửa import khá nhiều chỗ e test kĩ phần import và export
</commit_message>
<xml_diff>
--- a/public/upload/student_list_each_semester/2/D14_TH01.xlsx
+++ b/public/upload/student_list_each_semester/2/D14_TH01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\danh gia ren luyen thay hung\danh-sach-sinh-vien-cntt 2018\CNTT\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\danh gia ren luyen thay hung\danh-sach-sinh-vien-cntt 2018\CNTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="160">
   <si>
     <t>BỘ GIÁO DỤC VÀ ĐÀO TẠO</t>
   </si>
@@ -447,6 +447,15 @@
   </si>
   <si>
     <t>Tròn</t>
+  </si>
+  <si>
+    <t>DH51401593</t>
+  </si>
+  <si>
+    <t>Nguyễn Tuấn</t>
+  </si>
+  <si>
+    <t>Vỹ</t>
   </si>
   <si>
     <t>Lớp trưởng</t>
@@ -728,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -772,6 +781,10 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -784,61 +797,61 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1121,63 +1134,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="P44" sqref="P44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
     <col min="6" max="12" width="6.44140625" customWidth="1"/>
     <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
     </row>
     <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
     </row>
     <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -1186,76 +1198,76 @@
       <c r="D3" s="3"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
     </row>
     <row r="4" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
     </row>
     <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="22" t="s">
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
     </row>
@@ -1283,18 +1295,18 @@
       <c r="B8" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="27" t="s">
+      <c r="D8" s="30"/>
+      <c r="E8" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="32"/>
-      <c r="H8" s="33"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
       <c r="I8" s="25" t="s">
         <v>14</v>
       </c>
@@ -1320,9 +1332,9 @@
     <row r="9" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A9" s="26"/>
       <c r="B9" s="26"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="29"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="31"/>
       <c r="F9" s="8" t="s">
         <v>21</v>
       </c>
@@ -1347,10 +1359,10 @@
       <c r="B10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="35"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="9" t="s">
         <v>27</v>
       </c>
@@ -2303,96 +2315,106 @@
       <c r="N44" s="14"/>
       <c r="O44" s="14"/>
     </row>
-    <row r="45" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="4"/>
-      <c r="B45" s="36" t="s">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A45" s="10">
+        <v>35</v>
+      </c>
+      <c r="B45" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="C45" s="36"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="37" t="s">
+      <c r="C45" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="H45" s="37"/>
-      <c r="I45" s="37"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7" t="s">
+      <c r="D45" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="N45" s="7"/>
-      <c r="O45" s="7"/>
-    </row>
-    <row r="46" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="4"/>
-      <c r="B46" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="C46" s="36"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="H46" s="37"/>
-      <c r="I46" s="37"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="N46" s="7"/>
-      <c r="O46" s="7"/>
+      <c r="E45" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="14"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="16"/>
+      <c r="O46" s="16"/>
     </row>
     <row r="47" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
+      <c r="B47" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="23"/>
       <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
+      <c r="E47" s="7"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
+      <c r="G47" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
       <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
     </row>
     <row r="48" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
+      <c r="B48" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" s="23"/>
+      <c r="D48" s="4"/>
       <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
+      <c r="J48" s="4"/>
       <c r="K48" s="7"/>
       <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
+      <c r="M48" s="7" t="s">
+        <v>140</v>
+      </c>
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
     </row>
     <row r="49" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="7"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
       <c r="L49" s="7"/>
@@ -2401,12 +2423,10 @@
       <c r="O49" s="7"/>
     </row>
     <row r="50" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="A50" s="4"/>
       <c r="B50" s="7"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
@@ -2420,12 +2440,10 @@
       <c r="O50" s="7"/>
     </row>
     <row r="51" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="16" t="s">
-        <v>139</v>
-      </c>
+      <c r="A51" s="4"/>
       <c r="B51" s="7"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
@@ -2440,11 +2458,11 @@
     </row>
     <row r="52" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B52" s="7"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
@@ -2458,12 +2476,12 @@
       <c r="O52" s="7"/>
     </row>
     <row r="53" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>141</v>
+      <c r="A53" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="B53" s="7"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
@@ -2477,125 +2495,169 @@
       <c r="O53" s="7"/>
     </row>
     <row r="54" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="4"/>
-      <c r="B54" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15" t="s">
+      <c r="A54" s="4" t="s">
         <v>143</v>
       </c>
+      <c r="B54" s="7"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
-      <c r="G54" s="18" t="s">
-        <v>144</v>
-      </c>
+      <c r="G54" s="7"/>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
-      <c r="L54" s="17" t="s">
-        <v>145</v>
-      </c>
+      <c r="L54" s="7"/>
       <c r="M54" s="7"/>
       <c r="N54" s="7"/>
       <c r="O54" s="7"/>
     </row>
     <row r="55" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="4"/>
-      <c r="B55" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15" t="s">
-        <v>147</v>
-      </c>
+      <c r="A55" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B55" s="7"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
-      <c r="G55" s="18" t="s">
-        <v>148</v>
-      </c>
+      <c r="G55" s="7"/>
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
-      <c r="L55" s="7" t="s">
-        <v>149</v>
-      </c>
+      <c r="L55" s="7"/>
       <c r="M55" s="7"/>
       <c r="N55" s="7"/>
       <c r="O55" s="7"/>
     </row>
     <row r="56" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
-      <c r="B56" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15" t="s">
-        <v>151</v>
+      <c r="B56" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17" t="s">
+        <v>146</v>
       </c>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
-      <c r="G56" s="18" t="s">
-        <v>152</v>
+      <c r="G56" s="20" t="s">
+        <v>147</v>
       </c>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
-      <c r="L56" s="7" t="s">
-        <v>153</v>
+      <c r="L56" s="19" t="s">
+        <v>148</v>
       </c>
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
       <c r="O56" s="7"/>
     </row>
     <row r="57" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B57" s="7"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17" t="s">
+        <v>150</v>
+      </c>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
+      <c r="G57" s="20" t="s">
+        <v>151</v>
+      </c>
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
+      <c r="L57" s="7" t="s">
+        <v>152</v>
+      </c>
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
       <c r="O57" s="7"/>
     </row>
     <row r="58" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="B58" s="7"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17" t="s">
+        <v>154</v>
+      </c>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
+      <c r="G58" s="20" t="s">
+        <v>155</v>
+      </c>
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
-      <c r="L58" s="7"/>
+      <c r="L58" s="7" t="s">
+        <v>156</v>
+      </c>
       <c r="M58" s="7"/>
       <c r="N58" s="7"/>
       <c r="O58" s="7"/>
     </row>
+    <row r="59" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B59" s="7"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="7"/>
+    </row>
+    <row r="60" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B60" s="7"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:O1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:O2"/>
+    <mergeCell ref="G3:O3"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:H8"/>
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F5:M5"/>
@@ -2607,17 +2669,11 @@
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="N8:N9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:O1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:O2"/>
-    <mergeCell ref="G3:O3"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="G48:I48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ẩn nội dung ý kiến
</commit_message>
<xml_diff>
--- a/public/upload/student_list_each_semester/2/D14_TH01.xlsx
+++ b/public/upload/student_list_each_semester/2/D14_TH01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\danh gia ren luyen thay hung\danh-sach-sinh-vien-cntt 2018\CNTT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\desktop\ThucTap\danh gia ren luyen thay hung\danh-sach-sinh-vien-cntt 2018\CNTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,457 +71,457 @@
     <t>Khoa: Công Nghệ Thông Tin</t>
   </si>
   <si>
+    <t>Stt</t>
+  </si>
+  <si>
+    <t>MSSV</t>
+  </si>
+  <si>
+    <t>Họ và tên</t>
+  </si>
+  <si>
+    <t>Lớp</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Tổng điểm</t>
+  </si>
+  <si>
+    <t>Xếp loại</t>
+  </si>
+  <si>
+    <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>(1)</t>
+  </si>
+  <si>
+    <t>(2)</t>
+  </si>
+  <si>
+    <t>(3)</t>
+  </si>
+  <si>
+    <t>(4)</t>
+  </si>
+  <si>
+    <t>(5)</t>
+  </si>
+  <si>
+    <t>(6)</t>
+  </si>
+  <si>
+    <t>(7)</t>
+  </si>
+  <si>
+    <t>(8)</t>
+  </si>
+  <si>
+    <t>(9)</t>
+  </si>
+  <si>
+    <t>(10)</t>
+  </si>
+  <si>
+    <t>(11)</t>
+  </si>
+  <si>
+    <t>(12)</t>
+  </si>
+  <si>
+    <t>(13)</t>
+  </si>
+  <si>
+    <t>(14)</t>
+  </si>
+  <si>
+    <t>DH51400074</t>
+  </si>
+  <si>
+    <t>Ung Triệu</t>
+  </si>
+  <si>
+    <t>Biêu</t>
+  </si>
+  <si>
+    <t>D14_TH01</t>
+  </si>
+  <si>
+    <t>DH51400095</t>
+  </si>
+  <si>
+    <t>Quách Phú</t>
+  </si>
+  <si>
+    <t>Cường</t>
+  </si>
+  <si>
+    <t>DH51400153</t>
+  </si>
+  <si>
+    <t>Trịnh Công</t>
+  </si>
+  <si>
+    <t>Danh</t>
+  </si>
+  <si>
+    <t>DH51300213</t>
+  </si>
+  <si>
+    <t>Nguyễn Hoàng</t>
+  </si>
+  <si>
+    <t>Dũng</t>
+  </si>
+  <si>
+    <t>DH51400233</t>
+  </si>
+  <si>
+    <t>Phan Thành</t>
+  </si>
+  <si>
+    <t>Đạt</t>
+  </si>
+  <si>
+    <t>DH51400250</t>
+  </si>
+  <si>
+    <t>Thái Huỳnh</t>
+  </si>
+  <si>
+    <t>Đức</t>
+  </si>
+  <si>
+    <t>DH51400312</t>
+  </si>
+  <si>
+    <t>Huỳnh Gia</t>
+  </si>
+  <si>
+    <t>Hào</t>
+  </si>
+  <si>
+    <t>DH51400313</t>
+  </si>
+  <si>
+    <t>Lương Nhiêu</t>
+  </si>
+  <si>
+    <t>DH51400316</t>
+  </si>
+  <si>
+    <t>Nguyễn Duy</t>
+  </si>
+  <si>
+    <t>DH51400400</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn</t>
+  </si>
+  <si>
+    <t>Hiếu</t>
+  </si>
+  <si>
+    <t>DH51400453</t>
+  </si>
+  <si>
+    <t>Diệp Cẩm</t>
+  </si>
+  <si>
+    <t>Hòa</t>
+  </si>
+  <si>
+    <t>DH51400434</t>
+  </si>
+  <si>
+    <t>Nguyễn Minh</t>
+  </si>
+  <si>
+    <t>Hoàng</t>
+  </si>
+  <si>
+    <t>DH51400470</t>
+  </si>
+  <si>
+    <t>Đinh Quốc</t>
+  </si>
+  <si>
+    <t>Huy</t>
+  </si>
+  <si>
+    <t>DH51400475</t>
+  </si>
+  <si>
+    <t>Lê Gia</t>
+  </si>
+  <si>
+    <t>DH51401644</t>
+  </si>
+  <si>
+    <t>Nguyễn Mộc</t>
+  </si>
+  <si>
+    <t>Lâm</t>
+  </si>
+  <si>
+    <t>DH51400633</t>
+  </si>
+  <si>
+    <t>Trần Tuấn</t>
+  </si>
+  <si>
+    <t>Linh</t>
+  </si>
+  <si>
+    <t>DH51400592</t>
+  </si>
+  <si>
+    <t>Hồng Thành</t>
+  </si>
+  <si>
+    <t>Lộc</t>
+  </si>
+  <si>
+    <t>DH51400597</t>
+  </si>
+  <si>
+    <t>Nguyễn Vương Thành</t>
+  </si>
+  <si>
+    <t>DH51400871</t>
+  </si>
+  <si>
+    <t>Huỳnh Trọng</t>
+  </si>
+  <si>
+    <t>Nhân</t>
+  </si>
+  <si>
+    <t>DH51400948</t>
+  </si>
+  <si>
+    <t>Phát</t>
+  </si>
+  <si>
+    <t>DH51401026</t>
+  </si>
+  <si>
+    <t>Trần Hỷ</t>
+  </si>
+  <si>
+    <t>Phong</t>
+  </si>
+  <si>
+    <t>DH51400985</t>
+  </si>
+  <si>
+    <t>Lâm Hiệp</t>
+  </si>
+  <si>
+    <t>Phú</t>
+  </si>
+  <si>
+    <t>DH51400991</t>
+  </si>
+  <si>
+    <t>Võ Đình</t>
+  </si>
+  <si>
+    <t>DH51401033</t>
+  </si>
+  <si>
+    <t>Ô Kiếm</t>
+  </si>
+  <si>
+    <t>Quân</t>
+  </si>
+  <si>
+    <t>DH51401049</t>
+  </si>
+  <si>
+    <t>Hà Hải</t>
+  </si>
+  <si>
+    <t>Quốc</t>
+  </si>
+  <si>
+    <t>DH51401129</t>
+  </si>
+  <si>
+    <t>Phan Ngọc Minh</t>
+  </si>
+  <si>
+    <t>Tân</t>
+  </si>
+  <si>
+    <t>DH51401173</t>
+  </si>
+  <si>
+    <t>Phạm Quang</t>
+  </si>
+  <si>
+    <t>Thái</t>
+  </si>
+  <si>
+    <t>DH51401183</t>
+  </si>
+  <si>
+    <t>Dương Minh</t>
+  </si>
+  <si>
+    <t>Thành</t>
+  </si>
+  <si>
+    <t>DH51401191</t>
+  </si>
+  <si>
+    <t>Trần Minh</t>
+  </si>
+  <si>
+    <t>DH51401705</t>
+  </si>
+  <si>
+    <t>Nguyễn Trần Phước</t>
+  </si>
+  <si>
+    <t>Thiện</t>
+  </si>
+  <si>
+    <t>DH51401176</t>
+  </si>
+  <si>
+    <t>Lâm Chí</t>
+  </si>
+  <si>
+    <t>Thông</t>
+  </si>
+  <si>
+    <t>DH51401296</t>
+  </si>
+  <si>
+    <t>Trần Ngọc</t>
+  </si>
+  <si>
+    <t>Thuận</t>
+  </si>
+  <si>
+    <t>DH51401492</t>
+  </si>
+  <si>
+    <t>Võ Minh</t>
+  </si>
+  <si>
+    <t>Trí</t>
+  </si>
+  <si>
+    <t>DH51401462</t>
+  </si>
+  <si>
+    <t>Lê Văn</t>
+  </si>
+  <si>
+    <t>Tròn</t>
+  </si>
+  <si>
+    <t>DH51401593</t>
+  </si>
+  <si>
+    <t>Nguyễn Tuấn</t>
+  </si>
+  <si>
+    <t>Vỹ</t>
+  </si>
+  <si>
+    <t>Lớp trưởng</t>
+  </si>
+  <si>
+    <t>Bí thư chi đoàn</t>
+  </si>
+  <si>
+    <t>CVHT /GVCN</t>
+  </si>
+  <si>
+    <t>(Ký và ghi rõ họ tên)</t>
+  </si>
+  <si>
+    <t>Chú ý:</t>
+  </si>
+  <si>
+    <t>- Nhập thứ tự theo đúng danh sách sinh viên của Nhà trường.</t>
+  </si>
+  <si>
+    <t>- Cột (12) = (5) + (6) + (7) + (8) + (9) + (10)+(11)</t>
+  </si>
+  <si>
+    <t>- Cột (13) được xác định theo cột (12), cụ thể:</t>
+  </si>
+  <si>
+    <t>+ Từ 90 đến 100 điểm</t>
+  </si>
+  <si>
+    <t>: Xuất sắc;</t>
+  </si>
+  <si>
+    <t>+ Từ 50 đến dưới 65 điểm</t>
+  </si>
+  <si>
+    <t>: Trung bình;</t>
+  </si>
+  <si>
+    <t>+ Từ 80 đến dưới 90 điểm</t>
+  </si>
+  <si>
+    <t>: Tốt;</t>
+  </si>
+  <si>
+    <t>+ Từ 35 đến dưới 50 điểm</t>
+  </si>
+  <si>
+    <t>: Yếu;</t>
+  </si>
+  <si>
+    <t>+ Từ 65 đến dưới 80 điểm</t>
+  </si>
+  <si>
+    <t>: Khá;</t>
+  </si>
+  <si>
+    <t>+ Dưới 35 điểm</t>
+  </si>
+  <si>
+    <t>: Kém.</t>
+  </si>
+  <si>
+    <t>- Nếu SV không thực hiện Phiếu tự đánh giá thì để trống từ cột (5) đên cột (11), cột (12) ghi "0", cột (13) ghi "Kém", cột (14) ghi "*".</t>
+  </si>
+  <si>
+    <t>- Trước khi in nhớ xóa phần chú ý.</t>
+  </si>
+  <si>
     <t>Học kỳ: II</t>
-  </si>
-  <si>
-    <t>Stt</t>
-  </si>
-  <si>
-    <t>MSSV</t>
-  </si>
-  <si>
-    <t>Họ và tên</t>
-  </si>
-  <si>
-    <t>Lớp</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>II</t>
-  </si>
-  <si>
-    <t>III</t>
-  </si>
-  <si>
-    <t>IV</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>Tổng điểm</t>
-  </si>
-  <si>
-    <t>Xếp loại</t>
-  </si>
-  <si>
-    <t>Ghi chú</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>(1)</t>
-  </si>
-  <si>
-    <t>(2)</t>
-  </si>
-  <si>
-    <t>(3)</t>
-  </si>
-  <si>
-    <t>(4)</t>
-  </si>
-  <si>
-    <t>(5)</t>
-  </si>
-  <si>
-    <t>(6)</t>
-  </si>
-  <si>
-    <t>(7)</t>
-  </si>
-  <si>
-    <t>(8)</t>
-  </si>
-  <si>
-    <t>(9)</t>
-  </si>
-  <si>
-    <t>(10)</t>
-  </si>
-  <si>
-    <t>(11)</t>
-  </si>
-  <si>
-    <t>(12)</t>
-  </si>
-  <si>
-    <t>(13)</t>
-  </si>
-  <si>
-    <t>(14)</t>
-  </si>
-  <si>
-    <t>DH51400074</t>
-  </si>
-  <si>
-    <t>Ung Triệu</t>
-  </si>
-  <si>
-    <t>Biêu</t>
-  </si>
-  <si>
-    <t>D14_TH01</t>
-  </si>
-  <si>
-    <t>DH51400095</t>
-  </si>
-  <si>
-    <t>Quách Phú</t>
-  </si>
-  <si>
-    <t>Cường</t>
-  </si>
-  <si>
-    <t>DH51400153</t>
-  </si>
-  <si>
-    <t>Trịnh Công</t>
-  </si>
-  <si>
-    <t>Danh</t>
-  </si>
-  <si>
-    <t>DH51300213</t>
-  </si>
-  <si>
-    <t>Nguyễn Hoàng</t>
-  </si>
-  <si>
-    <t>Dũng</t>
-  </si>
-  <si>
-    <t>DH51400233</t>
-  </si>
-  <si>
-    <t>Phan Thành</t>
-  </si>
-  <si>
-    <t>Đạt</t>
-  </si>
-  <si>
-    <t>DH51400250</t>
-  </si>
-  <si>
-    <t>Thái Huỳnh</t>
-  </si>
-  <si>
-    <t>Đức</t>
-  </si>
-  <si>
-    <t>DH51400312</t>
-  </si>
-  <si>
-    <t>Huỳnh Gia</t>
-  </si>
-  <si>
-    <t>Hào</t>
-  </si>
-  <si>
-    <t>DH51400313</t>
-  </si>
-  <si>
-    <t>Lương Nhiêu</t>
-  </si>
-  <si>
-    <t>DH51400316</t>
-  </si>
-  <si>
-    <t>Nguyễn Duy</t>
-  </si>
-  <si>
-    <t>DH51400400</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn</t>
-  </si>
-  <si>
-    <t>Hiếu</t>
-  </si>
-  <si>
-    <t>DH51400453</t>
-  </si>
-  <si>
-    <t>Diệp Cẩm</t>
-  </si>
-  <si>
-    <t>Hòa</t>
-  </si>
-  <si>
-    <t>DH51400434</t>
-  </si>
-  <si>
-    <t>Nguyễn Minh</t>
-  </si>
-  <si>
-    <t>Hoàng</t>
-  </si>
-  <si>
-    <t>DH51400470</t>
-  </si>
-  <si>
-    <t>Đinh Quốc</t>
-  </si>
-  <si>
-    <t>Huy</t>
-  </si>
-  <si>
-    <t>DH51400475</t>
-  </si>
-  <si>
-    <t>Lê Gia</t>
-  </si>
-  <si>
-    <t>DH51401644</t>
-  </si>
-  <si>
-    <t>Nguyễn Mộc</t>
-  </si>
-  <si>
-    <t>Lâm</t>
-  </si>
-  <si>
-    <t>DH51400633</t>
-  </si>
-  <si>
-    <t>Trần Tuấn</t>
-  </si>
-  <si>
-    <t>Linh</t>
-  </si>
-  <si>
-    <t>DH51400592</t>
-  </si>
-  <si>
-    <t>Hồng Thành</t>
-  </si>
-  <si>
-    <t>Lộc</t>
-  </si>
-  <si>
-    <t>DH51400597</t>
-  </si>
-  <si>
-    <t>Nguyễn Vương Thành</t>
-  </si>
-  <si>
-    <t>DH51400871</t>
-  </si>
-  <si>
-    <t>Huỳnh Trọng</t>
-  </si>
-  <si>
-    <t>Nhân</t>
-  </si>
-  <si>
-    <t>DH51400948</t>
-  </si>
-  <si>
-    <t>Phát</t>
-  </si>
-  <si>
-    <t>DH51401026</t>
-  </si>
-  <si>
-    <t>Trần Hỷ</t>
-  </si>
-  <si>
-    <t>Phong</t>
-  </si>
-  <si>
-    <t>DH51400985</t>
-  </si>
-  <si>
-    <t>Lâm Hiệp</t>
-  </si>
-  <si>
-    <t>Phú</t>
-  </si>
-  <si>
-    <t>DH51400991</t>
-  </si>
-  <si>
-    <t>Võ Đình</t>
-  </si>
-  <si>
-    <t>DH51401033</t>
-  </si>
-  <si>
-    <t>Ô Kiếm</t>
-  </si>
-  <si>
-    <t>Quân</t>
-  </si>
-  <si>
-    <t>DH51401049</t>
-  </si>
-  <si>
-    <t>Hà Hải</t>
-  </si>
-  <si>
-    <t>Quốc</t>
-  </si>
-  <si>
-    <t>DH51401129</t>
-  </si>
-  <si>
-    <t>Phan Ngọc Minh</t>
-  </si>
-  <si>
-    <t>Tân</t>
-  </si>
-  <si>
-    <t>DH51401173</t>
-  </si>
-  <si>
-    <t>Phạm Quang</t>
-  </si>
-  <si>
-    <t>Thái</t>
-  </si>
-  <si>
-    <t>DH51401183</t>
-  </si>
-  <si>
-    <t>Dương Minh</t>
-  </si>
-  <si>
-    <t>Thành</t>
-  </si>
-  <si>
-    <t>DH51401191</t>
-  </si>
-  <si>
-    <t>Trần Minh</t>
-  </si>
-  <si>
-    <t>DH51401705</t>
-  </si>
-  <si>
-    <t>Nguyễn Trần Phước</t>
-  </si>
-  <si>
-    <t>Thiện</t>
-  </si>
-  <si>
-    <t>DH51401176</t>
-  </si>
-  <si>
-    <t>Lâm Chí</t>
-  </si>
-  <si>
-    <t>Thông</t>
-  </si>
-  <si>
-    <t>DH51401296</t>
-  </si>
-  <si>
-    <t>Trần Ngọc</t>
-  </si>
-  <si>
-    <t>Thuận</t>
-  </si>
-  <si>
-    <t>DH51401492</t>
-  </si>
-  <si>
-    <t>Võ Minh</t>
-  </si>
-  <si>
-    <t>Trí</t>
-  </si>
-  <si>
-    <t>DH51401462</t>
-  </si>
-  <si>
-    <t>Lê Văn</t>
-  </si>
-  <si>
-    <t>Tròn</t>
-  </si>
-  <si>
-    <t>DH51401593</t>
-  </si>
-  <si>
-    <t>Nguyễn Tuấn</t>
-  </si>
-  <si>
-    <t>Vỹ</t>
-  </si>
-  <si>
-    <t>Lớp trưởng</t>
-  </si>
-  <si>
-    <t>Bí thư chi đoàn</t>
-  </si>
-  <si>
-    <t>CVHT /GVCN</t>
-  </si>
-  <si>
-    <t>(Ký và ghi rõ họ tên)</t>
-  </si>
-  <si>
-    <t>Chú ý:</t>
-  </si>
-  <si>
-    <t>- Nhập thứ tự theo đúng danh sách sinh viên của Nhà trường.</t>
-  </si>
-  <si>
-    <t>- Cột (12) = (5) + (6) + (7) + (8) + (9) + (10)+(11)</t>
-  </si>
-  <si>
-    <t>- Cột (13) được xác định theo cột (12), cụ thể:</t>
-  </si>
-  <si>
-    <t>+ Từ 90 đến 100 điểm</t>
-  </si>
-  <si>
-    <t>: Xuất sắc;</t>
-  </si>
-  <si>
-    <t>+ Từ 50 đến dưới 65 điểm</t>
-  </si>
-  <si>
-    <t>: Trung bình;</t>
-  </si>
-  <si>
-    <t>+ Từ 80 đến dưới 90 điểm</t>
-  </si>
-  <si>
-    <t>: Tốt;</t>
-  </si>
-  <si>
-    <t>+ Từ 35 đến dưới 50 điểm</t>
-  </si>
-  <si>
-    <t>: Yếu;</t>
-  </si>
-  <si>
-    <t>+ Từ 65 đến dưới 80 điểm</t>
-  </si>
-  <si>
-    <t>: Khá;</t>
-  </si>
-  <si>
-    <t>+ Dưới 35 điểm</t>
-  </si>
-  <si>
-    <t>: Kém.</t>
-  </si>
-  <si>
-    <t>- Nếu SV không thực hiện Phiếu tự đánh giá thì để trống từ cột (5) đên cột (11), cột (12) ghi "0", cột (13) ghi "Kém", cột (14) ghi "*".</t>
-  </si>
-  <si>
-    <t>- Trước khi in nhớ xóa phần chú ý.</t>
   </si>
   <si>
     <t>Năm học: 2017 - 2018</t>
@@ -797,6 +797,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -807,51 +852,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1140,138 +1140,138 @@
       <selection activeCell="F6" sqref="F6:M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="6.44140625" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="6.453125" customWidth="1"/>
+    <col min="13" max="13" width="19.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="27" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+    </row>
+    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.35">
+      <c r="A2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="37" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-    </row>
-    <row r="4" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+    </row>
+    <row r="4" spans="1:15" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-    </row>
-    <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28" t="s">
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27" t="s">
+      <c r="C6" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="7"/>
       <c r="C7" s="4"/>
@@ -1288,130 +1288,130 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:15" ht="15" x14ac:dyDescent="0.35">
+      <c r="A8" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="C8" s="29" t="s">
         <v>10</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>11</v>
       </c>
       <c r="D8" s="30"/>
       <c r="E8" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="33" t="s">
         <v>12</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>13</v>
       </c>
       <c r="G8" s="34"/>
       <c r="H8" s="35"/>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="25" t="s">
+      <c r="K8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="L8" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="25" t="s">
+      <c r="M8" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="25" t="s">
+      <c r="N8" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="25" t="s">
+      <c r="O8" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="31"/>
       <c r="D9" s="32"/>
       <c r="E9" s="31"/>
       <c r="F9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="H9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="B10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="C10" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="D10" s="37"/>
+      <c r="E10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="9" t="s">
+      <c r="F10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="J10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="K10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="L10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="M10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="N10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="O10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="O10" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>1</v>
       </c>
       <c r="B11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="D11" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>40</v>
-      </c>
       <c r="E11" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -1424,21 +1424,21 @@
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>2</v>
       </c>
       <c r="B12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="D12" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>44</v>
-      </c>
       <c r="E12" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -1451,21 +1451,21 @@
       <c r="N12" s="14"/>
       <c r="O12" s="14"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
         <v>3</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="D13" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>47</v>
-      </c>
       <c r="E13" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
@@ -1478,21 +1478,21 @@
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
         <v>4</v>
       </c>
       <c r="B14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="D14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>50</v>
-      </c>
       <c r="E14" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
@@ -1505,21 +1505,21 @@
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
         <v>5</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="D15" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>53</v>
-      </c>
       <c r="E15" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
@@ -1532,21 +1532,21 @@
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
         <v>6</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="D16" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>56</v>
-      </c>
       <c r="E16" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -1559,21 +1559,21 @@
       <c r="N16" s="14"/>
       <c r="O16" s="14"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
         <v>7</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="D17" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="E17" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
@@ -1586,21 +1586,21 @@
       <c r="N17" s="14"/>
       <c r="O17" s="14"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
         <v>8</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>61</v>
-      </c>
       <c r="D18" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
@@ -1613,21 +1613,21 @@
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
         <v>9</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>63</v>
-      </c>
       <c r="D19" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
@@ -1640,21 +1640,21 @@
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
         <v>10</v>
       </c>
       <c r="B20" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="D20" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>66</v>
-      </c>
       <c r="E20" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
@@ -1667,21 +1667,21 @@
       <c r="N20" s="14"/>
       <c r="O20" s="14"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
         <v>11</v>
       </c>
       <c r="B21" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="D21" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>69</v>
-      </c>
       <c r="E21" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
@@ -1694,21 +1694,21 @@
       <c r="N21" s="14"/>
       <c r="O21" s="14"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="10">
         <v>12</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="D22" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>72</v>
-      </c>
       <c r="E22" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -1721,21 +1721,21 @@
       <c r="N22" s="14"/>
       <c r="O22" s="14"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="10">
         <v>13</v>
       </c>
       <c r="B23" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="D23" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="13" t="s">
-        <v>75</v>
-      </c>
       <c r="E23" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -1748,21 +1748,21 @@
       <c r="N23" s="14"/>
       <c r="O23" s="14"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
         <v>14</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>77</v>
-      </c>
       <c r="D24" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -1775,21 +1775,21 @@
       <c r="N24" s="14"/>
       <c r="O24" s="14"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="10">
         <v>15</v>
       </c>
       <c r="B25" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="D25" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>80</v>
-      </c>
       <c r="E25" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
@@ -1802,21 +1802,21 @@
       <c r="N25" s="14"/>
       <c r="O25" s="14"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="10">
         <v>16</v>
       </c>
       <c r="B26" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="D26" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>83</v>
-      </c>
       <c r="E26" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -1829,21 +1829,21 @@
       <c r="N26" s="14"/>
       <c r="O26" s="14"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="10">
         <v>17</v>
       </c>
       <c r="B27" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="D27" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="E27" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1856,21 +1856,21 @@
       <c r="N27" s="14"/>
       <c r="O27" s="14"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="10">
         <v>18</v>
       </c>
       <c r="B28" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>88</v>
-      </c>
       <c r="D28" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
@@ -1883,21 +1883,21 @@
       <c r="N28" s="14"/>
       <c r="O28" s="14"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
         <v>19</v>
       </c>
       <c r="B29" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="D29" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="13" t="s">
-        <v>91</v>
-      </c>
       <c r="E29" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
@@ -1910,21 +1910,21 @@
       <c r="N29" s="14"/>
       <c r="O29" s="14"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="10">
         <v>20</v>
       </c>
       <c r="B30" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>93</v>
-      </c>
       <c r="E30" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
@@ -1937,21 +1937,21 @@
       <c r="N30" s="14"/>
       <c r="O30" s="14"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="10">
         <v>21</v>
       </c>
       <c r="B31" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="D31" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="D31" s="13" t="s">
-        <v>96</v>
-      </c>
       <c r="E31" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -1964,21 +1964,21 @@
       <c r="N31" s="14"/>
       <c r="O31" s="14"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
         <v>22</v>
       </c>
       <c r="B32" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="D32" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D32" s="13" t="s">
-        <v>99</v>
-      </c>
       <c r="E32" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
@@ -1991,21 +1991,21 @@
       <c r="N32" s="14"/>
       <c r="O32" s="14"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="10">
         <v>23</v>
       </c>
       <c r="B33" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>101</v>
-      </c>
       <c r="D33" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
@@ -2018,21 +2018,21 @@
       <c r="N33" s="14"/>
       <c r="O33" s="14"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="10">
         <v>24</v>
       </c>
       <c r="B34" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="D34" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="13" t="s">
-        <v>104</v>
-      </c>
       <c r="E34" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
@@ -2045,21 +2045,21 @@
       <c r="N34" s="14"/>
       <c r="O34" s="14"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="10">
         <v>25</v>
       </c>
       <c r="B35" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="D35" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="13" t="s">
-        <v>107</v>
-      </c>
       <c r="E35" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
@@ -2072,21 +2072,21 @@
       <c r="N35" s="14"/>
       <c r="O35" s="14"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="10">
         <v>26</v>
       </c>
       <c r="B36" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="D36" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D36" s="13" t="s">
-        <v>110</v>
-      </c>
       <c r="E36" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
@@ -2099,21 +2099,21 @@
       <c r="N36" s="14"/>
       <c r="O36" s="14"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="10">
         <v>27</v>
       </c>
       <c r="B37" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="D37" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D37" s="13" t="s">
-        <v>113</v>
-      </c>
       <c r="E37" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
@@ -2126,21 +2126,21 @@
       <c r="N37" s="14"/>
       <c r="O37" s="14"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" s="10">
         <v>28</v>
       </c>
       <c r="B38" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="D38" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="D38" s="13" t="s">
-        <v>116</v>
-      </c>
       <c r="E38" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
@@ -2153,21 +2153,21 @@
       <c r="N38" s="14"/>
       <c r="O38" s="14"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" s="10">
         <v>29</v>
       </c>
       <c r="B39" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C39" s="12" t="s">
-        <v>118</v>
-      </c>
       <c r="D39" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F39" s="14"/>
       <c r="G39" s="14"/>
@@ -2180,21 +2180,21 @@
       <c r="N39" s="14"/>
       <c r="O39" s="14"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" s="10">
         <v>30</v>
       </c>
       <c r="B40" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="D40" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D40" s="13" t="s">
-        <v>121</v>
-      </c>
       <c r="E40" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
@@ -2207,21 +2207,21 @@
       <c r="N40" s="14"/>
       <c r="O40" s="14"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" s="10">
         <v>31</v>
       </c>
       <c r="B41" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="D41" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D41" s="13" t="s">
-        <v>124</v>
-      </c>
       <c r="E41" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F41" s="14"/>
       <c r="G41" s="14"/>
@@ -2234,21 +2234,21 @@
       <c r="N41" s="14"/>
       <c r="O41" s="14"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" s="10">
         <v>32</v>
       </c>
       <c r="B42" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="D42" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="D42" s="13" t="s">
-        <v>127</v>
-      </c>
       <c r="E42" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F42" s="14"/>
       <c r="G42" s="14"/>
@@ -2261,21 +2261,21 @@
       <c r="N42" s="14"/>
       <c r="O42" s="14"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" s="10">
         <v>33</v>
       </c>
       <c r="B43" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="D43" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="D43" s="13" t="s">
-        <v>130</v>
-      </c>
       <c r="E43" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
@@ -2288,21 +2288,21 @@
       <c r="N43" s="14"/>
       <c r="O43" s="14"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" s="10">
         <v>34</v>
       </c>
       <c r="B44" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C44" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="D44" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D44" s="13" t="s">
-        <v>133</v>
-      </c>
       <c r="E44" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
@@ -2315,21 +2315,21 @@
       <c r="N44" s="14"/>
       <c r="O44" s="14"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" s="10">
         <v>35</v>
       </c>
       <c r="B45" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="D45" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="D45" s="13" t="s">
-        <v>136</v>
-      </c>
       <c r="E45" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
@@ -2342,7 +2342,7 @@
       <c r="N45" s="14"/>
       <c r="O45" s="14"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -2359,53 +2359,53 @@
       <c r="N46" s="16"/>
       <c r="O46" s="16"/>
     </row>
-    <row r="47" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="4"/>
-      <c r="B47" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="C47" s="23"/>
+      <c r="B47" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47" s="38"/>
       <c r="D47" s="4"/>
       <c r="E47" s="7"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="H47" s="24"/>
-      <c r="I47" s="24"/>
+      <c r="G47" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="H47" s="39"/>
+      <c r="I47" s="39"/>
       <c r="J47" s="4"/>
       <c r="K47" s="7"/>
       <c r="L47" s="7"/>
       <c r="M47" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N47" s="7"/>
       <c r="O47" s="7"/>
     </row>
-    <row r="48" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="4"/>
-      <c r="B48" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="C48" s="23"/>
+      <c r="B48" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" s="38"/>
       <c r="D48" s="4"/>
       <c r="E48" s="7"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
+      <c r="G48" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="H48" s="39"/>
+      <c r="I48" s="39"/>
       <c r="J48" s="4"/>
       <c r="K48" s="7"/>
       <c r="L48" s="7"/>
       <c r="M48" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
     </row>
-    <row r="49" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="4"/>
       <c r="B49" s="7"/>
       <c r="C49" s="17"/>
@@ -2422,7 +2422,7 @@
       <c r="N49" s="7"/>
       <c r="O49" s="7"/>
     </row>
-    <row r="50" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="4"/>
       <c r="B50" s="7"/>
       <c r="C50" s="17"/>
@@ -2439,7 +2439,7 @@
       <c r="N50" s="7"/>
       <c r="O50" s="7"/>
     </row>
-    <row r="51" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="4"/>
       <c r="B51" s="7"/>
       <c r="C51" s="17"/>
@@ -2456,9 +2456,9 @@
       <c r="N51" s="7"/>
       <c r="O51" s="7"/>
     </row>
-    <row r="52" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="17"/>
@@ -2475,9 +2475,9 @@
       <c r="N52" s="7"/>
       <c r="O52" s="7"/>
     </row>
-    <row r="53" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="17"/>
@@ -2494,9 +2494,9 @@
       <c r="N53" s="7"/>
       <c r="O53" s="7"/>
     </row>
-    <row r="54" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B54" s="7"/>
       <c r="C54" s="17"/>
@@ -2513,9 +2513,9 @@
       <c r="N54" s="7"/>
       <c r="O54" s="7"/>
     </row>
-    <row r="55" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="17"/>
@@ -2532,84 +2532,84 @@
       <c r="N55" s="7"/>
       <c r="O55" s="7"/>
     </row>
-    <row r="56" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="4"/>
       <c r="B56" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C56" s="17"/>
       <c r="D56" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
       <c r="L56" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
       <c r="O56" s="7"/>
     </row>
-    <row r="57" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="4"/>
       <c r="B57" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C57" s="17"/>
       <c r="D57" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
       <c r="G57" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
       <c r="L57" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
       <c r="O57" s="7"/>
     </row>
-    <row r="58" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A58" s="4"/>
       <c r="B58" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C58" s="17"/>
       <c r="D58" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
       <c r="G58" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
       <c r="L58" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M58" s="7"/>
       <c r="N58" s="7"/>
       <c r="O58" s="7"/>
     </row>
-    <row r="59" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B59" s="7"/>
       <c r="C59" s="17"/>
@@ -2626,9 +2626,9 @@
       <c r="N59" s="7"/>
       <c r="O59" s="7"/>
     </row>
-    <row r="60" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A60" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="17"/>
@@ -2647,17 +2647,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:O1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:O2"/>
-    <mergeCell ref="G3:O3"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="G48:I48"/>
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F5:M5"/>
@@ -2669,11 +2663,17 @@
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="N8:N9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:O1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:O2"/>
+    <mergeCell ref="G3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sửa width input chấm điểm. thêm chặn 12
</commit_message>
<xml_diff>
--- a/public/upload/student_list_each_semester/2/D14_TH01.xlsx
+++ b/public/upload/student_list_each_semester/2/D14_TH01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\desktop\ThucTap\danh gia ren luyen thay hung\danh-sach-sinh-vien-cntt 2018\CNTT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\danh gia ren luyen thay hung\danh-sach-sinh-vien-cntt 2018\CNTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,6 +71,9 @@
     <t>Khoa: Công Nghệ Thông Tin</t>
   </si>
   <si>
+    <t>Học kỳ: II</t>
+  </si>
+  <si>
     <t>Stt</t>
   </si>
   <si>
@@ -519,9 +522,6 @@
   </si>
   <si>
     <t>- Trước khi in nhớ xóa phần chú ý.</t>
-  </si>
-  <si>
-    <t>Học kỳ: II</t>
   </si>
   <si>
     <t>Năm học: 2017 - 2018</t>
@@ -797,61 +797,61 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1140,138 +1140,138 @@
       <selection activeCell="F6" sqref="F6:M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="6.453125" customWidth="1"/>
-    <col min="13" max="13" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="6.44140625" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-    </row>
-    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-    </row>
-    <row r="4" spans="1:15" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+    </row>
+    <row r="4" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-    </row>
-    <row r="5" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24" t="s">
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23" t="s">
+      <c r="C6" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="7"/>
       <c r="C7" s="4"/>
@@ -1288,130 +1288,130 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="1:15" ht="15" x14ac:dyDescent="0.35">
-      <c r="A8" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="27" t="s">
+    <row r="8" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="25" t="s">
         <v>9</v>
       </c>
+      <c r="B8" s="25" t="s">
+        <v>10</v>
+      </c>
       <c r="C8" s="29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="30"/>
       <c r="E8" s="29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G8" s="34"/>
       <c r="H8" s="35"/>
-      <c r="I8" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="27" t="s">
+      <c r="I8" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="J8" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="K8" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="27" t="s">
+      <c r="L8" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="27" t="s">
+      <c r="M8" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="O8" s="27" t="s">
+      <c r="N8" s="25" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
+      <c r="O8" s="25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="31"/>
       <c r="D9" s="32"/>
       <c r="E9" s="31"/>
       <c r="F9" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="37"/>
+      <c r="C10" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="22"/>
       <c r="E10" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>1</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -1424,21 +1424,21 @@
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>2</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -1451,21 +1451,21 @@
       <c r="N12" s="14"/>
       <c r="O12" s="14"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>3</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
@@ -1478,21 +1478,21 @@
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>4</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
@@ -1505,21 +1505,21 @@
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>5</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
@@ -1532,21 +1532,21 @@
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>6</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -1559,21 +1559,21 @@
       <c r="N16" s="14"/>
       <c r="O16" s="14"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>7</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
@@ -1586,21 +1586,21 @@
       <c r="N17" s="14"/>
       <c r="O17" s="14"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>8</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>58</v>
-      </c>
       <c r="E18" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
@@ -1613,21 +1613,21 @@
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>9</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
@@ -1640,21 +1640,21 @@
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>10</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
@@ -1667,21 +1667,21 @@
       <c r="N20" s="14"/>
       <c r="O20" s="14"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>11</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
@@ -1694,21 +1694,21 @@
       <c r="N21" s="14"/>
       <c r="O21" s="14"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>12</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -1721,21 +1721,21 @@
       <c r="N22" s="14"/>
       <c r="O22" s="14"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <v>13</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -1748,21 +1748,21 @@
       <c r="N23" s="14"/>
       <c r="O23" s="14"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>14</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>74</v>
-      </c>
       <c r="E24" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -1775,21 +1775,21 @@
       <c r="N24" s="14"/>
       <c r="O24" s="14"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <v>15</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
@@ -1802,21 +1802,21 @@
       <c r="N25" s="14"/>
       <c r="O25" s="14"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>16</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -1829,21 +1829,21 @@
       <c r="N26" s="14"/>
       <c r="O26" s="14"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <v>17</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1856,21 +1856,21 @@
       <c r="N27" s="14"/>
       <c r="O27" s="14"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <v>18</v>
       </c>
       <c r="B28" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>85</v>
-      </c>
       <c r="E28" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
@@ -1883,21 +1883,21 @@
       <c r="N28" s="14"/>
       <c r="O28" s="14"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>19</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
@@ -1910,21 +1910,21 @@
       <c r="N29" s="14"/>
       <c r="O29" s="14"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <v>20</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
@@ -1937,21 +1937,21 @@
       <c r="N30" s="14"/>
       <c r="O30" s="14"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
         <v>21</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -1964,21 +1964,21 @@
       <c r="N31" s="14"/>
       <c r="O31" s="14"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="10">
         <v>22</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
@@ -1991,21 +1991,21 @@
       <c r="N32" s="14"/>
       <c r="O32" s="14"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="10">
         <v>23</v>
       </c>
       <c r="B33" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>98</v>
-      </c>
       <c r="E33" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
@@ -2018,21 +2018,21 @@
       <c r="N33" s="14"/>
       <c r="O33" s="14"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="10">
         <v>24</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
@@ -2045,21 +2045,21 @@
       <c r="N34" s="14"/>
       <c r="O34" s="14"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="10">
         <v>25</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
@@ -2072,21 +2072,21 @@
       <c r="N35" s="14"/>
       <c r="O35" s="14"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="10">
         <v>26</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
@@ -2099,21 +2099,21 @@
       <c r="N36" s="14"/>
       <c r="O36" s="14"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="10">
         <v>27</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
@@ -2126,21 +2126,21 @@
       <c r="N37" s="14"/>
       <c r="O37" s="14"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="10">
         <v>28</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
@@ -2153,21 +2153,21 @@
       <c r="N38" s="14"/>
       <c r="O38" s="14"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="10">
         <v>29</v>
       </c>
       <c r="B39" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D39" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>115</v>
-      </c>
       <c r="E39" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F39" s="14"/>
       <c r="G39" s="14"/>
@@ -2180,21 +2180,21 @@
       <c r="N39" s="14"/>
       <c r="O39" s="14"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="10">
         <v>30</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
@@ -2207,21 +2207,21 @@
       <c r="N40" s="14"/>
       <c r="O40" s="14"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="10">
         <v>31</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F41" s="14"/>
       <c r="G41" s="14"/>
@@ -2234,21 +2234,21 @@
       <c r="N41" s="14"/>
       <c r="O41" s="14"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="10">
         <v>32</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F42" s="14"/>
       <c r="G42" s="14"/>
@@ -2261,21 +2261,21 @@
       <c r="N42" s="14"/>
       <c r="O42" s="14"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="10">
         <v>33</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
@@ -2288,21 +2288,21 @@
       <c r="N43" s="14"/>
       <c r="O43" s="14"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="10">
         <v>34</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
@@ -2315,21 +2315,21 @@
       <c r="N44" s="14"/>
       <c r="O44" s="14"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="10">
         <v>35</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
@@ -2342,7 +2342,7 @@
       <c r="N45" s="14"/>
       <c r="O45" s="14"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -2359,53 +2359,53 @@
       <c r="N46" s="16"/>
       <c r="O46" s="16"/>
     </row>
-    <row r="47" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
-      <c r="B47" s="38" t="s">
-        <v>136</v>
-      </c>
-      <c r="C47" s="38"/>
+      <c r="B47" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="23"/>
       <c r="D47" s="4"/>
       <c r="E47" s="7"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="39" t="s">
-        <v>137</v>
-      </c>
-      <c r="H47" s="39"/>
-      <c r="I47" s="39"/>
+      <c r="G47" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
       <c r="J47" s="4"/>
       <c r="K47" s="7"/>
       <c r="L47" s="7"/>
       <c r="M47" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="N47" s="7"/>
       <c r="O47" s="7"/>
     </row>
-    <row r="48" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
-      <c r="B48" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="C48" s="38"/>
+      <c r="B48" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" s="23"/>
       <c r="D48" s="4"/>
       <c r="E48" s="7"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="H48" s="39"/>
-      <c r="I48" s="39"/>
+      <c r="G48" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
       <c r="J48" s="4"/>
       <c r="K48" s="7"/>
       <c r="L48" s="7"/>
       <c r="M48" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
     </row>
-    <row r="49" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="7"/>
       <c r="C49" s="17"/>
@@ -2422,7 +2422,7 @@
       <c r="N49" s="7"/>
       <c r="O49" s="7"/>
     </row>
-    <row r="50" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="7"/>
       <c r="C50" s="17"/>
@@ -2439,7 +2439,7 @@
       <c r="N50" s="7"/>
       <c r="O50" s="7"/>
     </row>
-    <row r="51" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="7"/>
       <c r="C51" s="17"/>
@@ -2456,9 +2456,9 @@
       <c r="N51" s="7"/>
       <c r="O51" s="7"/>
     </row>
-    <row r="52" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="17"/>
@@ -2475,9 +2475,9 @@
       <c r="N52" s="7"/>
       <c r="O52" s="7"/>
     </row>
-    <row r="53" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="17"/>
@@ -2494,9 +2494,9 @@
       <c r="N53" s="7"/>
       <c r="O53" s="7"/>
     </row>
-    <row r="54" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B54" s="7"/>
       <c r="C54" s="17"/>
@@ -2513,9 +2513,9 @@
       <c r="N54" s="7"/>
       <c r="O54" s="7"/>
     </row>
-    <row r="55" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="17"/>
@@ -2532,84 +2532,84 @@
       <c r="N55" s="7"/>
       <c r="O55" s="7"/>
     </row>
-    <row r="56" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="19" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C56" s="17"/>
       <c r="D56" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
       <c r="L56" s="19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
       <c r="O56" s="7"/>
     </row>
-    <row r="57" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C57" s="17"/>
       <c r="D57" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
       <c r="G57" s="20" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
       <c r="L57" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
       <c r="O57" s="7"/>
     </row>
-    <row r="58" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="20" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C58" s="17"/>
       <c r="D58" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
       <c r="G58" s="20" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
       <c r="L58" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M58" s="7"/>
       <c r="N58" s="7"/>
       <c r="O58" s="7"/>
     </row>
-    <row r="59" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B59" s="7"/>
       <c r="C59" s="17"/>
@@ -2626,9 +2626,9 @@
       <c r="N59" s="7"/>
       <c r="O59" s="7"/>
     </row>
-    <row r="60" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="17"/>
@@ -2647,11 +2647,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:O1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:O2"/>
+    <mergeCell ref="G3:O3"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:H8"/>
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F5:M5"/>
@@ -2663,17 +2669,11 @@
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="N8:N9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:O1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:O2"/>
-    <mergeCell ref="G3:O3"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="G48:I48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>